<commit_message>
Add broken link test card in index.html and update selenium script to handle missing URLs for error tests
</commit_message>
<xml_diff>
--- a/link_check_report.xlsx
+++ b/link_check_report.xlsx
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.surveymonkey.com</t>
+          <t>https://www.rbi.org.in</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -466,7 +466,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.google.com</t>
+          <t>https://www.owasp.org</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -486,7 +486,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.owasp.org</t>
+          <t>https://www.sebi.gov.in</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -526,7 +526,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.sebi.gov.in</t>
+          <t>https://www.surveymonkey.com</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -546,7 +546,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.rbi.org.in</t>
+          <t>https://www.google.com</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>